<commit_message>
* [hunglv] make function for SS
</commit_message>
<xml_diff>
--- a/src/main/resources/ReportTemplate/DSTV - Du Tru.xlsx
+++ b/src/main/resources/ReportTemplate/DSTV - Du Tru.xlsx
@@ -13,7 +13,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'02-2017'!#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'02-2017'!$6:$7</definedName>
   </definedNames>
-  <calcPr calcId="144525" fullCalcOnLoad="1" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -38,9 +38,6 @@
     <t>Ngày rời tàu</t>
   </si>
   <si>
-    <t>Có</t>
-  </si>
-  <si>
     <t>Không</t>
   </si>
   <si>
@@ -85,6 +82,9 @@
   <si>
     <t>Kế hoạch TV 
 trong  tháng 01</t>
+  </si>
+  <si>
+    <t>Có</t>
   </si>
 </sst>
 </file>
@@ -92,7 +92,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="193" formatCode="[$-409]d/mmm/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d/mmm/yyyy;@"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -210,7 +210,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="193" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -636,7 +636,7 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -649,7 +649,8 @@
     <col min="6" max="6" width="10.875" style="2" customWidth="1"/>
     <col min="7" max="7" width="13.25" style="2" customWidth="1"/>
     <col min="8" max="8" width="14.75" style="1" hidden="1" customWidth="1"/>
-    <col min="9" max="10" width="6.625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="13.25" style="2" customWidth="1"/>
+    <col min="10" max="10" width="6.625" style="2" customWidth="1"/>
     <col min="11" max="11" width="12.875" style="3" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="9.375" style="2" customWidth="1"/>
     <col min="13" max="14" width="8.75" style="2"/>
@@ -659,7 +660,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C1" s="28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D1" s="28"/>
       <c r="E1" s="28"/>
@@ -669,7 +670,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C2" s="28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
@@ -682,7 +683,7 @@
       <c r="A4" s="4"/>
       <c r="B4" s="13"/>
       <c r="C4" s="29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="29"/>
       <c r="E4" s="29"/>
@@ -710,12 +711,12 @@
       <c r="K5" s="10"/>
       <c r="L5" s="10"/>
       <c r="M5" s="30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N5" s="30"/>
       <c r="O5" s="15">
         <f ca="1">TODAY()</f>
-        <v>43380</v>
+        <v>43467</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -735,26 +736,26 @@
         <v>5</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G6" s="25"/>
       <c r="H6" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I6" s="26" t="s">
         <v>4</v>
       </c>
       <c r="J6" s="26"/>
       <c r="K6" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="L6" s="25" t="s">
         <v>10</v>
-      </c>
-      <c r="L6" s="25" t="s">
-        <v>11</v>
       </c>
       <c r="M6" s="25"/>
       <c r="N6" s="25"/>
       <c r="O6" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -764,27 +765,27 @@
       <c r="D7" s="25"/>
       <c r="E7" s="25"/>
       <c r="F7" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="16" t="s">
         <v>8</v>
-      </c>
-      <c r="G7" s="16" t="s">
-        <v>9</v>
       </c>
       <c r="H7" s="21"/>
       <c r="I7" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="16" t="s">
         <v>6</v>
-      </c>
-      <c r="J7" s="16" t="s">
-        <v>7</v>
       </c>
       <c r="K7" s="27"/>
       <c r="L7" s="16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M7" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="N7" s="16" t="s">
         <v>12</v>
-      </c>
-      <c r="N7" s="16" t="s">
-        <v>13</v>
       </c>
       <c r="O7" s="25"/>
     </row>
@@ -797,7 +798,7 @@
       <c r="F8" s="18"/>
       <c r="G8" s="17"/>
       <c r="H8" s="5"/>
-      <c r="I8" s="6"/>
+      <c r="I8" s="17"/>
       <c r="J8" s="7"/>
       <c r="K8" s="22"/>
       <c r="L8" s="6"/>
@@ -915,6 +916,7 @@
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
       <c r="H17" s="8"/>
+      <c r="I17" s="9"/>
       <c r="J17" s="9"/>
       <c r="K17" s="23"/>
       <c r="O17" s="1"/>
@@ -965,12 +967,12 @@
     <mergeCell ref="C2:I2"/>
     <mergeCell ref="C4:O4"/>
     <mergeCell ref="M5:N5"/>
+    <mergeCell ref="F6:G6"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:G6"/>
   </mergeCells>
   <pageMargins left="0.48" right="0.48" top="0.17" bottom="0.16" header="0.11" footer="0.16"/>
   <pageSetup paperSize="9" scale="63" orientation="landscape" r:id="rId1"/>

</xml_diff>